<commit_message>
Creacion de preguntas, tematicas, modulos y actualizacion en oficinas
</commit_message>
<xml_diff>
--- a/Documentos/tablas.xlsx
+++ b/Documentos/tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SIRC\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD93EF2D-C1D0-475E-A2C1-7E27946D39CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C420EF21-C65F-4DC9-8471-A373ACEB71F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-2475" windowWidth="29040" windowHeight="15840" xr2:uid="{C006E4AF-046C-4101-A2A3-3510E6ECAF9F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="72">
   <si>
     <t>sucusarles</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>no va</t>
   </si>
 </sst>
 </file>
@@ -494,6 +497,45 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -507,45 +549,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -869,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACE899F-1EF2-456A-979F-3702F3951232}">
-  <dimension ref="B2:AB56"/>
+  <dimension ref="A2:AB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,6 +907,12 @@
       <c r="E2" t="s">
         <v>70</v>
       </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" t="s">
+        <v>70</v>
+      </c>
       <c r="N2" t="s">
         <v>70</v>
       </c>
@@ -912,38 +921,38 @@
       </c>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="E3" s="49" t="s">
+      <c r="C3" s="44"/>
+      <c r="E3" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="49"/>
-      <c r="H3" s="50" t="s">
+      <c r="F3" s="45"/>
+      <c r="H3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="K3" s="35" t="s">
+      <c r="I3" s="46"/>
+      <c r="K3" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="35"/>
-      <c r="N3" s="46" t="s">
+      <c r="L3" s="48"/>
+      <c r="N3" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="46"/>
-      <c r="T3" s="42" t="s">
+      <c r="O3" s="42"/>
+      <c r="T3" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="42"/>
-      <c r="X3" s="36" t="s">
+      <c r="U3" s="38"/>
+      <c r="X3" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="Y3" s="36"/>
-      <c r="AA3" s="37" t="s">
+      <c r="Y3" s="49"/>
+      <c r="AA3" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="AB3" s="37"/>
+      <c r="AB3" s="50"/>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1364,30 +1373,30 @@
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="52" t="s">
+      <c r="E16" s="35" t="s">
         <v>70</v>
       </c>
       <c r="K16" s="16"/>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B17" s="51" t="s">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B17" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="E17" s="47" t="s">
+      <c r="C17" s="47"/>
+      <c r="E17" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="47"/>
-      <c r="H17" s="43" t="s">
+      <c r="F17" s="43"/>
+      <c r="H17" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="43"/>
-      <c r="K17" s="44" t="s">
+      <c r="I17" s="39"/>
+      <c r="K17" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="L17" s="44"/>
-    </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="L17" s="40"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="s">
         <v>24</v>
       </c>
@@ -1416,7 +1425,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
@@ -1441,12 +1450,12 @@
       <c r="L19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="AA19" s="38" t="s">
+      <c r="AA19" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="AB19" s="38"/>
-    </row>
-    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AB19" s="51"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
@@ -1474,7 +1483,7 @@
       </c>
       <c r="AB20" s="32"/>
     </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>12</v>
       </c>
@@ -1504,7 +1513,7 @@
       </c>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>23</v>
       </c>
@@ -1540,7 +1549,7 @@
       </c>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="2:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>28</v>
       </c>
@@ -1568,10 +1577,10 @@
       <c r="L23" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="T23" s="39" t="s">
+      <c r="T23" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="U23" s="39"/>
+      <c r="U23" s="52"/>
       <c r="V23" s="24" t="s">
         <v>56</v>
       </c>
@@ -1580,7 +1589,10 @@
       </c>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
       <c r="B24" s="27" t="s">
         <v>30</v>
       </c>
@@ -1621,7 +1633,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
       <c r="B25" s="27" t="s">
         <v>31</v>
       </c>
@@ -1658,7 +1673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
         <v>34</v>
       </c>
@@ -1690,7 +1705,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>13</v>
       </c>
@@ -1717,7 +1732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>15</v>
       </c>
@@ -1744,7 +1759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -1768,23 +1783,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="E30" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="45"/>
+      <c r="F30" s="41"/>
       <c r="T30" s="33" t="s">
         <v>5</v>
       </c>
       <c r="U30" s="33"/>
     </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>18</v>
       </c>
@@ -1807,7 +1822,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>19</v>
       </c>
@@ -1848,10 +1863,10 @@
       </c>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="41"/>
+      <c r="C35" s="37"/>
       <c r="E35" s="10" t="s">
         <v>13</v>
       </c>
@@ -1986,10 +2001,10 @@
       </c>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="40"/>
+      <c r="C47" s="36"/>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
@@ -2065,6 +2080,10 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AA19:AB19"/>
+    <mergeCell ref="T23:U23"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="T3:U3"/>
@@ -2078,10 +2097,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AA19:AB19"/>
-    <mergeCell ref="T23:U23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>